<commit_message>
Partial data upon running scraper on D_SearchTerms; program terminated early
</commit_message>
<xml_diff>
--- a/Keywords.xlsx
+++ b/Keywords.xlsx
@@ -1,12 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mitalibafna/Desktop/CodeSwitching/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" tabRatio="500"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -274,10 +290,6 @@
     <t>सियासत</t>
   </si>
   <si>
-    <t xml:space="preserve">Dalit Panthers
-</t>
-  </si>
-  <si>
     <t>vote bank</t>
   </si>
   <si>
@@ -810,43 +822,50 @@
   </si>
   <si>
     <t>atrocities</t>
+  </si>
+  <si>
+    <t>Dalit Panthers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <name val="Times New Roman"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <name val="Times New Roman"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF454545"/>
       <name val="Times New Roman"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
     </font>
-    <font/>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="&quot;Times New Roman&quot;"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF212121"/>
       <name val="Times New Roman"/>
     </font>
@@ -856,7 +875,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -866,60 +885,320 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:J89"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -936,7 +1215,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -953,7 +1232,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -970,7 +1249,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -987,7 +1266,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -1004,7 +1283,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -1021,7 +1300,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
@@ -1038,7 +1317,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
@@ -1055,7 +1334,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>31</v>
       </c>
@@ -1072,7 +1351,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>35</v>
       </c>
@@ -1089,7 +1368,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
@@ -1106,7 +1385,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>43</v>
       </c>
@@ -1123,7 +1402,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>47</v>
       </c>
@@ -1140,7 +1419,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>51</v>
       </c>
@@ -1157,7 +1436,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>55</v>
       </c>
@@ -1173,7 +1452,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>59</v>
       </c>
@@ -1189,7 +1468,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>63</v>
       </c>
@@ -1205,7 +1484,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>67</v>
       </c>
@@ -1221,7 +1500,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>71</v>
       </c>
@@ -1238,7 +1517,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>75</v>
       </c>
@@ -1255,7 +1534,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>79</v>
       </c>
@@ -1272,7 +1551,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>83</v>
       </c>
@@ -1289,793 +1568,793 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>87</v>
+        <v>265</v>
       </c>
       <c r="B23" s="2"/>
       <c r="D23" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E23" s="2"/>
       <c r="G23" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H23" s="2"/>
       <c r="J23" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="B24" s="2"/>
       <c r="D24" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E24" s="2"/>
       <c r="G24" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H24" s="2"/>
       <c r="J24" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="B25" s="2"/>
       <c r="D25" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E25" s="2"/>
       <c r="G25" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H25" s="2"/>
       <c r="J25" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="B26" s="2"/>
       <c r="D26" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E26" s="2"/>
       <c r="G26" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H26" s="2"/>
       <c r="J26" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="B27" s="2"/>
       <c r="D27" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E27" s="2"/>
       <c r="G27" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H27" s="2"/>
       <c r="J27" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="B28" s="2"/>
       <c r="D28" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E28" s="2"/>
       <c r="G28" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H28" s="2"/>
       <c r="J28" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="B29" s="2"/>
       <c r="D29" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E29" s="2"/>
       <c r="G29" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H29" s="2"/>
       <c r="J29" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="3" t="s">
-        <v>115</v>
       </c>
       <c r="B30" s="2"/>
       <c r="D30" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E30" s="2"/>
       <c r="G30" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H30" s="2"/>
       <c r="J30" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="3" t="s">
-        <v>119</v>
       </c>
       <c r="B31" s="2"/>
       <c r="D31" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E31" s="2"/>
       <c r="G31" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H31" s="2"/>
       <c r="J31" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="4" t="s">
-        <v>123</v>
       </c>
       <c r="B32" s="2"/>
       <c r="D32" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E32" s="2"/>
       <c r="G32" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H32" s="2"/>
       <c r="J32" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="33">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B33" s="2"/>
       <c r="D33" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E33" s="2"/>
       <c r="G33" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H33" s="2"/>
       <c r="J33" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
         <v>129</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="3" t="s">
-        <v>130</v>
       </c>
       <c r="B34" s="2"/>
       <c r="D34" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E34" s="2"/>
       <c r="G34" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H34" s="2"/>
       <c r="J34" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="4" t="s">
-        <v>134</v>
       </c>
       <c r="B35" s="2"/>
       <c r="D35" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E35" s="2"/>
       <c r="G35" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H35" s="2"/>
       <c r="J35" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
         <v>137</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="3" t="s">
-        <v>138</v>
       </c>
       <c r="B36" s="2"/>
       <c r="D36" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E36" s="2"/>
       <c r="G36" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H36" s="2"/>
       <c r="J36" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="3" t="s">
-        <v>142</v>
       </c>
       <c r="B37" s="2"/>
       <c r="D37" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E37" s="2"/>
       <c r="G37" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H37" s="2"/>
       <c r="J37" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
         <v>145</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="5" t="s">
-        <v>146</v>
       </c>
       <c r="B38" s="2"/>
       <c r="D38" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E38" s="2"/>
       <c r="G38" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H38" s="2"/>
       <c r="J38" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
         <v>149</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="B39" s="2"/>
       <c r="D39" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E39" s="2"/>
       <c r="G39" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H39" s="2"/>
       <c r="J39" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="3" t="s">
+      <c r="D40" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>155</v>
       </c>
       <c r="E40" s="2"/>
       <c r="G40" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H40" s="2"/>
       <c r="J40" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="3" t="s">
+      <c r="D41" s="3" t="s">
         <v>158</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>159</v>
       </c>
       <c r="E41" s="2"/>
       <c r="G41" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H41" s="2"/>
       <c r="J41" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="3" t="s">
+      <c r="D42" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="E42" s="2"/>
       <c r="G42" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="J42" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="J42" s="3" t="s">
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="5" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="5" t="s">
+      <c r="D43" s="3" t="s">
         <v>166</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>167</v>
       </c>
       <c r="E43" s="2"/>
       <c r="G43" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="J43" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="J43" s="3" t="s">
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="3" t="s">
+      <c r="D44" s="4" t="s">
         <v>170</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>171</v>
       </c>
       <c r="E44" s="2"/>
       <c r="G44" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="J44" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="J44" s="3" t="s">
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
         <v>173</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="3" t="s">
-        <v>174</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="6"/>
       <c r="D45" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E45" s="2"/>
       <c r="J45" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
         <v>176</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="3" t="s">
-        <v>177</v>
       </c>
       <c r="B46" s="2"/>
       <c r="D46" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E46" s="2"/>
       <c r="J46" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="3" t="s">
+      <c r="D47" s="4" t="s">
         <v>180</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>181</v>
       </c>
       <c r="E47" s="2"/>
       <c r="J47" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="3" t="s">
+      <c r="D48" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="J48" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="J48" s="3" t="s">
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="3" t="s">
+      <c r="D49" s="3" t="s">
         <v>186</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>187</v>
       </c>
       <c r="E49" s="2"/>
       <c r="J49" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="3" t="s">
+      <c r="D50" s="3" t="s">
         <v>189</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>190</v>
       </c>
       <c r="E50" s="2"/>
       <c r="J50" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="3" t="s">
+      <c r="D51" s="3" t="s">
         <v>192</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>193</v>
       </c>
       <c r="E51" s="2"/>
       <c r="J51" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D52" s="3" t="s">
         <v>194</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="D52" s="3" t="s">
-        <v>195</v>
       </c>
       <c r="E52" s="2"/>
       <c r="J52" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D53" s="3" t="s">
         <v>196</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="D53" s="3" t="s">
-        <v>197</v>
       </c>
       <c r="E53" s="2"/>
       <c r="J53" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D54" s="3" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="54">
-      <c r="D54" s="3" t="s">
+      <c r="J54" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="J54" s="3" t="s">
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D55" s="3" t="s">
         <v>200</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="D55" s="3" t="s">
-        <v>201</v>
       </c>
       <c r="E55" s="2"/>
       <c r="J55" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D56" s="3" t="s">
         <v>202</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="D56" s="3" t="s">
-        <v>203</v>
       </c>
       <c r="E56" s="2"/>
       <c r="J56" s="3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="57">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="7"/>
       <c r="D57" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E57" s="2"/>
       <c r="J57" s="3" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="58">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="7"/>
       <c r="D58" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E58" s="3"/>
       <c r="J58" s="3" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="59">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="7"/>
       <c r="D59" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="J59" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="J59" s="3" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="60">
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="7"/>
       <c r="D60" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E60" s="2"/>
       <c r="J60" s="3" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="61">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="7"/>
       <c r="D61" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E61" s="2"/>
       <c r="J61" s="3" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="62">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="7"/>
       <c r="D62" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="J62" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="J62" s="3" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="63">
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="7"/>
       <c r="D63" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="J63" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="J63" s="3" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="64">
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="7"/>
       <c r="D64" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="J64" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="J64" s="3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="65">
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="7"/>
       <c r="D65" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E65" s="2"/>
       <c r="J65" s="3" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="66">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="7"/>
       <c r="D66" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E66" s="2"/>
       <c r="J66" s="3" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="67">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="7"/>
       <c r="D67" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E67" s="2"/>
       <c r="J67" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="68">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="7"/>
       <c r="D68" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E68" s="2"/>
       <c r="J68" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="69">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="7"/>
       <c r="D69" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E69" s="2"/>
       <c r="J69" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="70">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="7"/>
       <c r="D70" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E70" s="2"/>
       <c r="J70" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="71">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="7"/>
       <c r="D71" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E71" s="2"/>
       <c r="J71" s="3" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="72">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="7"/>
       <c r="D72" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E72" s="2"/>
       <c r="J72" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D73" s="3" t="s">
         <v>236</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="D73" s="3" t="s">
-        <v>237</v>
       </c>
       <c r="E73" s="2"/>
       <c r="J73" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D74" s="3" t="s">
         <v>238</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="D74" s="3" t="s">
-        <v>239</v>
       </c>
       <c r="E74" s="2"/>
       <c r="J74" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D75" s="3" t="s">
         <v>240</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="D75" s="3" t="s">
-        <v>241</v>
       </c>
       <c r="E75" s="2"/>
       <c r="J75" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D76" s="3" t="s">
         <v>242</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="D76" s="3" t="s">
-        <v>243</v>
       </c>
       <c r="E76" s="2"/>
       <c r="J76" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D77" s="3" t="s">
         <v>244</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="D77" s="3" t="s">
-        <v>245</v>
       </c>
       <c r="E77" s="2"/>
       <c r="J77" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D78" s="3" t="s">
         <v>246</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="D78" s="3" t="s">
-        <v>247</v>
       </c>
       <c r="E78" s="2"/>
       <c r="J78" s="3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D79" s="3" t="s">
         <v>248</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="D79" s="3" t="s">
-        <v>249</v>
       </c>
       <c r="E79" s="2"/>
       <c r="J79" s="3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D80" s="3" t="s">
         <v>250</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="D80" s="3" t="s">
-        <v>251</v>
       </c>
       <c r="E80" s="2"/>
       <c r="J80" s="3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="81" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D81" s="3" t="s">
         <v>252</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="D81" s="3" t="s">
-        <v>253</v>
       </c>
       <c r="E81" s="2"/>
       <c r="J81" s="3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="82" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D82" s="3" t="s">
         <v>254</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="D82" s="3" t="s">
-        <v>255</v>
       </c>
       <c r="E82" s="2"/>
       <c r="J82" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="83" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D83" s="3" t="s">
         <v>256</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="D83" s="3" t="s">
-        <v>257</v>
       </c>
       <c r="E83" s="2"/>
       <c r="J83" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="84" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D84" s="3" t="s">
         <v>258</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="D84" s="3" t="s">
-        <v>259</v>
       </c>
       <c r="E84" s="2"/>
       <c r="J84" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="85" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D85" s="3" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="85">
-      <c r="D85" s="3" t="s">
+      <c r="E85" s="2"/>
+    </row>
+    <row r="86" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D86" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="E85" s="2"/>
-    </row>
-    <row r="86">
-      <c r="D86" s="3" t="s">
+    </row>
+    <row r="87" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D87" s="3" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="87">
-      <c r="D87" s="3" t="s">
+    <row r="88" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D88" s="3" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="88">
-      <c r="D88" s="3" t="s">
+    <row r="89" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D89" s="3" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="89">
-      <c r="D89" s="3" t="s">
-        <v>265</v>
-      </c>
-    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>